<commit_message>
Aggiunte latitudine e longitudine fermate e stazioni
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8EFECDC-0EDE-42DB-93E3-C5485056758F}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60ED3A43-DE8E-40B5-9B56-18951CCDEDCC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Bergamo</t>
   </si>
@@ -65,12 +65,21 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -132,11 +141,22 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.00000000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0.00000000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -190,13 +210,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8480836-BEC5-47AE-8239-7E57A485AE3C}" name="Tabella1" displayName="Tabella1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D5" xr:uid="{C8480836-BEC5-47AE-8239-7E57A485AE3C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2B3696EE-3666-48E1-9DF5-50F71AF4F39D}" name="name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{554944E7-EE90-4500-8DF2-A47D9A7CB08A}" name="address" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{DBE2C48A-D9A4-4794-974D-E4DBC7D7C423}" name="town" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{3D666FF5-63D6-4EBD-85A8-B30407C94A7F}" name="province" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C8480836-BEC5-47AE-8239-7E57A485AE3C}" name="Tabella1" displayName="Tabella1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F5" xr:uid="{C8480836-BEC5-47AE-8239-7E57A485AE3C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2B3696EE-3666-48E1-9DF5-50F71AF4F39D}" name="name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{554944E7-EE90-4500-8DF2-A47D9A7CB08A}" name="address" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DBE2C48A-D9A4-4794-974D-E4DBC7D7C423}" name="town" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{3D666FF5-63D6-4EBD-85A8-B30407C94A7F}" name="province" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{4D6DE96E-CF8B-45E1-A4A4-2879FA2C647E}" name="lat" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82D87D68-71A4-4569-8E7F-EE95E2F46532}" name="lon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -465,9 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -475,9 +499,11 @@
     <col min="2" max="2" width="24.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -490,8 +516,14 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -504,8 +536,14 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="6">
+        <v>45.7007227</v>
+      </c>
+      <c r="F2" s="6">
+        <v>9.6650854000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -518,8 +556,14 @@
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6">
+        <v>45.703040399999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>9.6651491000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -532,8 +576,14 @@
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="6">
+        <v>45.7065403</v>
+      </c>
+      <c r="F4" s="6">
+        <v>9.6580069000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -546,62 +596,68 @@
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6">
+        <v>45.703340500000003</v>
+      </c>
+      <c r="F5" s="6">
+        <v>9.6645737999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
aggiunta metodi nella classe QueryDB per gestire il recupero dei dati dai database
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60ED3A43-DE8E-40B5-9B56-18951CCDEDCC}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B98F0013-EF31-431B-A6DF-EEA390E44B27}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.00000000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +138,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -150,11 +147,11 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.00000000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="0.00000000"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -490,7 +487,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +513,10 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -536,10 +533,10 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>45.7007227</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>9.6650854000000006</v>
       </c>
     </row>
@@ -556,10 +553,10 @@
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>45.703040399999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>9.6651491000000007</v>
       </c>
     </row>
@@ -576,10 +573,10 @@
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>45.7065403</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>9.6580069000000002</v>
       </c>
     </row>
@@ -596,10 +593,10 @@
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>45.703340500000003</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>9.6645737999999994</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificata gestione DB e aggiunta dei mezzi sulla mappa
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B98F0013-EF31-431B-A6DF-EEA390E44B27}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65AF300E-20F8-4203-B839-2C607BAC9D7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Bergamo</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>45.708509</t>
+  </si>
+  <si>
+    <t>9.650654</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,11 +599,11 @@
       <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
-        <v>45.703340500000003</v>
-      </c>
-      <c r="F5" s="4">
-        <v>9.6645737999999994</v>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sistemazione controlli relativi alla creazione dei database
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/funicular_station_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65AF300E-20F8-4203-B839-2C607BAC9D7A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{66E7F05E-6563-41D4-AB78-2501F611F0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87CC55CE-F69E-49F0-8011-46D8F74E4344}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>